<commit_message>
Add reference to Default form value.xlsx
</commit_message>
<xml_diff>
--- a/Document/Reports/Report 5/Staff contract & compensation test cases.xlsx
+++ b/Document/Reports/Report 5/Staff contract & compensation test cases.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="101">
   <si>
     <t>2.1 &lt;Staff&gt; View Contracts</t>
   </si>
@@ -104,34 +104,9 @@
     <t>A contract with status is "Pending" created successfully</t>
   </si>
   <si>
-    <t>Create Customer
-Create Contract</t>
-  </si>
-  <si>
     <t>A message notify this vehicle plate number is existed in the system</t>
   </si>
   <si>
-    <t>1. Create customer "Nguyen Van A" has customer code is KH0001
-2. Click create new contract, input form is displayed
-3. Fill out the form with customer code is KH0001
-4. Set contract start date to 12 July 2015
-5. Click submit button</t>
-  </si>
-  <si>
-    <t>1. Create customer "Nguyen Van A" has customer code is KH0001
-2. Click create new contract, input form is displayed
-3. Fill out the form with customer code is KH0001
-4. Set contract start date to 21 July 2015
-5. Click submit button</t>
-  </si>
-  <si>
-    <t>1. Create customer "Nguyen Van A" has customer code is KH0001, customer "Duong Thien Hoa" has customer code is KH0002
-2. Create new contract with start date is 12 July 2015, contract status is Ready, vehicle plate number is 59Y9-38482
-3. Click create new contract, input form is displayed
-4. Fill out the form with vehicle plate number is 59Y9-38482
-5. Click submit button</t>
-  </si>
-  <si>
     <t>Create contract fail because of existed vehicle plate number</t>
   </si>
   <si>
@@ -159,22 +134,10 @@
     <t>Renew contract success</t>
   </si>
   <si>
-    <t>Create Contract</t>
-  </si>
-  <si>
-    <t>Create Contract
-View Contracts</t>
-  </si>
-  <si>
     <t>Renew contract fail because of contract term is out of bound</t>
   </si>
   <si>
     <t>Renew contract success with request for new card and delivery it</t>
-  </si>
-  <si>
-    <t>Create Contract
-Print Card
-View Contracts</t>
   </si>
   <si>
     <t>Create contract fail because of there are no customer</t>
@@ -199,28 +162,10 @@
     <t>Search contract with customer name</t>
   </si>
   <si>
-    <t>1. Create 3 customer with names "Dang Van Ngu", "Duong Tu Ky" and "Nguyen Dinh Bao" alternatively
-2. Create 2 contract HD0001 and HD0002 belongs to "Dang Van Ngu" and "Nguyen Dinh Bao" in turn
-3. Input "Nguyen Dinh Bao" to search box
-4. Click search button</t>
-  </si>
-  <si>
     <t>Display contract HD0002 in the grid view</t>
   </si>
   <si>
     <t>Search contract with no keyword</t>
-  </si>
-  <si>
-    <t>1. Create 3 customer with names "Dang Van Ngu", "Duong Tu Ky" and "Nguyen Dinh Bao" alternatively
-2. Create 2 contract HD0001 and HD0002 belongs to "Dang Van Ngu" and "Nguyen Dinh Bao" in turn
-3. Click search button</t>
-  </si>
-  <si>
-    <t>1. Create customer "Nguyen Van A" has customer code is KH0001
-2. Click create new contract, input form is displayed
-3. Fill out the form with customer code is KH0002
-4. Set contract start date to 12 July 2015
-5. Click submit button</t>
   </si>
   <si>
     <t>Renew contract successfully, its status is "No card".
@@ -248,53 +193,6 @@
     <t>Cancel contract having "Ready" status</t>
   </si>
   <si>
-    <t>1. Create new contract has start date is 6 July 2015, expired date is 12 July 2015. Contract status is "Expired"
-2. Click view this contract detail
-3. Click renew contract button, renew contract form displayed
-4. Fill out the form, set expired date to 13 July 2016
-5. Check request for new card box
-6. Click submit button</t>
-  </si>
-  <si>
-    <t>1. Create new contract has start date is 6 July 2015, expired date is 12 August 2015. Contract status is "No card"
-2. Click view this contract detail
-3. Click renew contract button, renew contract form displayed
-4. Fill out the form, set expired date to 13 December 2016
-5. Click submit button</t>
-  </si>
-  <si>
-    <t>1. Create new contract has start date is 6 July 2015, expired date is 12 July 2015. Contract status is "Expired"
-2. Click view this contract detail
-3. Click renew contract button, renew contract form displayed
-4. Fill out the form, set expired date to 13 July 2016
-5. Click submit button</t>
-  </si>
-  <si>
-    <t>1. Create new contract has start date is 9 July 2015, expired date is 13 August 2015. Contract status is "No card"
-2. Print a card with code "12-34-56-78-91" for this contract. Contract new status is "Ready"
-3. Click view this contract detail
-4. Click renew contract button, renew contract form displayed button
-5. Fill out the form, set expired date to 13 August 2016
-6. Check request new card box
-7. Check delivery this card box
-8. Click submit button</t>
-  </si>
-  <si>
-    <t>1. Create new contract has start date is 10 July 2015, expired date is 1 September 2015. Contract status is "No card"
-2. Click view this contract detail
-3. Click renew contract button, renew contract form displayed
-4. Fill out the form, set expired date to 1 September 2016
-5. Click submit button</t>
-  </si>
-  <si>
-    <t>1. Create new contract has start date is 11 July 2015, expired date is 11 July 2016. Contract status is "No card"
-2. Print a card with code "12-34-56-78-AZ" for this contract. Contract new status is "Ready"
-3. Click view this contract detail
-4. Click cancel contract button, cancel contract form displayed
-5. Fill out the form
-6. Click submit button</t>
-  </si>
-  <si>
     <t>Cancel contract successfully, its status is "Cancelled".
 The card with code "12-34-56-78-AZ" is deactivated</t>
   </si>
@@ -311,19 +209,6 @@
     <t>A message notify cancel reason is can not empty, request Staff to fill it out</t>
   </si>
   <si>
-    <t>1. Create new contract has start date is 11 July 2015, expired date is 11 July 2016. Contract status is "No card"
-2. Click view this contract detail
-3. Click cancel contract button, cancel contract form displayed
-4. Click submit button</t>
-  </si>
-  <si>
-    <t>1. Create new contract has start date is 11 July 2015, expired date is 11 July 2016. Contract status is "Request cancel"
-2. Click view this contract detail
-3. Click handle cancel contract request button, cancel contract form displayed
-4. Select cancel this contract, fill out the form
-5. Click submit button</t>
-  </si>
-  <si>
     <t>WCL1</t>
   </si>
   <si>
@@ -340,10 +225,6 @@
   </si>
   <si>
     <t>View compensation list</t>
-  </si>
-  <si>
-    <t>Create Contract
-Create Compensation</t>
   </si>
   <si>
     <t>1. Create new contract with code is "HD0001"
@@ -363,17 +244,6 @@
     <t>A message notify there are no value for this search</t>
   </si>
   <si>
-    <t>1. Create 2 new contract with code is "HD0001", "HD0002"
-2. Create 4 new compensation, 2 for each contract
-3. Input "HD0001" to search box
-4. Click search button</t>
-  </si>
-  <si>
-    <t>1. Create 2 new contract with code is "HD0001", "HD0002"
-2. Create 4 new compensation, 2 for each contract
-3. Click search button</t>
-  </si>
-  <si>
     <t>View an unsolved compensation detail</t>
   </si>
   <si>
@@ -381,11 +251,6 @@
   </si>
   <si>
     <t>View an solved compensation detail</t>
-  </si>
-  <si>
-    <t>Create Contract
-Create Compensation
-Resolve Compensation</t>
   </si>
   <si>
     <t>1. Create new contract
@@ -399,18 +264,176 @@
 4. Click compensation code to view its detail</t>
   </si>
   <si>
-    <t>Display compensation detail page with solve compensation information</t>
-  </si>
-  <si>
     <t>Resolve compensation success</t>
+  </si>
+  <si>
+    <t>1. Create new contract has start date is 6 July 2015, expired date is 12 July 2015. Contract status is "Expired"
+2. Click view this contract detail
+3. Click "Gia hạn" button, renew contract form displayed
+4. Fill out the form:
+- Gia hạn đến: 13/08/2016
+- Ngày nộp phí:  13/07/2015
+5. Click submit button</t>
+  </si>
+  <si>
+    <t>1. Create new contract has start date is 6 July 2015, expired date is 12 August 2015. Contract status is "No card"
+2. Click view this contract detail
+3. Click "Gia hạn" button, renew contract form displayed
+4. Fill out the form:
+- Gia hạn đến: 13/12/2016
+- Ngày nộp phí:  13/07/2015
+5. Click "Gia hạn hợp đồng" button</t>
+  </si>
+  <si>
+    <t>1. Create new contract has start date is 6 July 2015, expired date is 12 July 2015. Contract status is "Expired"
+2. Click view this contract detail
+3. Click "Gia hạn" button, renew contract form displayed
+4. Fill out the form:
+- Gia hạn đến: 13/08/2016
+- Ngày nộp phí:  13/07/2015
+5. Check "Cấp thẻ mới" box
+6. Click "Gia hạn hợp đồng" button</t>
+  </si>
+  <si>
+    <t>1. Create new contract has start date is 9 July 2015, expired date is 13 August 2015. Contract status is "No card"
+2. Print a card with code "12-34-56-78-91" for this contract. Contract new status is "Ready"
+3. Click view this contract detail
+4. Click "Gia hạn" button, renew contract form displayed button
+5. Fill out the form:
+- Gia hạn đến: 13/08/2016
+- Ngày nộp phí:  13/07/2015
+6. Check "Cấp thẻ mới", "Vận chuyển thẻ" boxes
+7. Click "Gia hạn hợp đồng" button</t>
+  </si>
+  <si>
+    <t>1. Create new contract has start date is 10 July 2015, expired date is 1 September 2015. Contract status is "No card"
+2. Click view this contract detail
+3. Click "Gia hạn" button, renew contract form displayed
+4. Fill out the form:
+- Gia hạn đến: 01/09/2016
+- Ngày nộp phí:  13/07/2015
+5. Click "Gia hạn hợp đồng" button</t>
+  </si>
+  <si>
+    <t>1. Create customer "Nguyen Van A" has customer code is KH0001
+2. Click create new contract, input form is displayed
+3. Input all default value according to "Default_value_for_forms.xlsx" file, customer code is KH0002
+4. Set contract start date to 12 July 2015
+5. Click "Tạo hợp đồng" button</t>
+  </si>
+  <si>
+    <t>1. Create customer "Nguyen Van A" has customer code is KH0001, customer "Duong Thien Hoa" has customer code is KH0002
+2. Create new contract with start date is 12 July 2015, contract status is Ready, vehicle plate number is 59Y9-38482
+3. Click create new contract, input form is displayed
+4. Input all default value according to "Default_value_for_forms.xlsx" file
+5. Set vehicle plate number is 59Y9-38482
+6. Click "Tạo hợp đồng" button</t>
+  </si>
+  <si>
+    <t>1. Create customer "Nguyen Van A" has customer code is KH0001
+2. Click create new contract, input form is displayed
+3. Input all default value according to "Default_value_for_forms.xlsx" file
+4. Set customer code is KH0001, contract start date to 21 July 2015
+5. Click "Tạo hợp đồng" button</t>
+  </si>
+  <si>
+    <t>1. Create customer "Nguyen Van A" has customer code is KH0001
+2. Click create new contract, input form is displayed
+3. Input all default value according to "Default_value_for_forms.xlsx" file
+4. Set customer code is KH0001, contract start date to 12 July 2015
+5. Click "Tạo hợp đồng" button</t>
+  </si>
+  <si>
+    <t>1. Create 3 customer with names "Dang Van Ngu", "Duong Tu Ky" and "Nguyen Dinh Bao" alternatively
+2. Create 2 contract HD0001 and HD0002 belongs to "Dang Van Ngu" and "Nguyen Dinh Bao" in turn
+3. Input "Nguyen Dinh Bao" to search box
+4. Click "Tìm kiếm" button</t>
+  </si>
+  <si>
+    <t>1. Create 3 customer with names "Dang Van Ngu", "Duong Tu Ky" and "Nguyen Dinh Bao" alternatively
+2. Create 2 contract HD0001 and HD0002 belongs to "Dang Van Ngu" and "Nguyen Dinh Bao" in turn
+3. Click "Tìm kiếm" button</t>
+  </si>
+  <si>
+    <t>1. Create 2 new contract with code is "HD0001", "HD0002"
+2. Create 4 new compensation, 2 for each contract
+3. Input "HD0001" to search box
+4. Click "Tìm kiếm" button</t>
+  </si>
+  <si>
+    <t>1. Create 2 new contract with code is "HD0001", "HD0002"
+2. Create 4 new compensation, 2 for each contract
+3. Click "Tìm kiếm" button</t>
+  </si>
+  <si>
+    <t>1. Create new contract has start date is 11 July 2015, expired date is 11 July 2016. Contract status is "No card"
+2. Click view this contract detail
+3. Click "Hủy hợp đồng" button, cancel contract form displayed
+4. Click "Đồng ý hủy" button</t>
+  </si>
+  <si>
+    <t>1. Create new contract has start date is 11 July 2015, expired date is 11 July 2016. Contract status is "No card"
+2. Print a card with code "12-34-56-78-AZ" for this contract. Contract new status is "Ready"
+3. Click view this contract detail
+4. Click "Hủy hợp đồng" button, cancel contract form displayed
+5. Fill out the form:
+- Ngày hủy hợp đồng: 13/07/2015
+- Lý do hủy hợp đồng: Mất xe
+6. Click "Đồng ý hủy" button</t>
+  </si>
+  <si>
+    <t>CC1- Create Contract
+Create Compensation</t>
+  </si>
+  <si>
+    <t>CC1 - Create Contract</t>
+  </si>
+  <si>
+    <t>Create Customer
+CC1 - Create Contract</t>
+  </si>
+  <si>
+    <t>CC1 - Create Contract
+Create Compensation</t>
+  </si>
+  <si>
+    <t>CC1 - Create Contract
+Create Compensation
+RC1 - Resolve Compensation</t>
+  </si>
+  <si>
+    <t>CC1 - Create Contract
+WC1 - View Contracts</t>
+  </si>
+  <si>
+    <t>CC1 - Create Contract
+Print Card
+WC1 - View Contracts</t>
+  </si>
+  <si>
+    <t>CC1 - Create Contract
+PC1 - Print Card
+WC1 - View Contracts</t>
   </si>
   <si>
     <t>1. Create new contract
 2. Create new compensation for this contract
 3. Click compensation code in list of compensation
-4. Click resolve this compensation request button, solve form is displayed
-5. Fill out the form, select "Từ chối bồi thường"
-6. Click submit button</t>
+4. Click "Giải quyết yêu cầu" button, solve form is displayed
+5. Fill out the form:
+- Ngày giải quyết yêu cầu: 13/07/2015
+- Quyết định của công ty: "Từ chối bồi thường"
+6. Click "Quyết định" button</t>
+  </si>
+  <si>
+    <t>Display compensation detail page with solved compensation information</t>
+  </si>
+  <si>
+    <t>1. Create new contract has start date is 11 July 2015, expired date is 11 July 2016. Contract status is "Request cancel"
+2. Click view this contract detail
+3. Click handle cancel contract request button, cancel contract form displayed
+4. Quyết định của công ty: Hủy hợp đồng này
+5. Click "Xác nhận" button</t>
   </si>
 </sst>
 </file>
@@ -799,15 +822,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="29.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="64.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1" bestFit="1" customWidth="1"/>
@@ -852,19 +875,19 @@
         <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G3" s="6">
         <v>42198</v>
@@ -876,19 +899,19 @@
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G4" s="6">
         <v>42198</v>
@@ -900,19 +923,19 @@
         <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G5" s="6">
         <v>42198</v>
@@ -952,15 +975,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>22</v>
@@ -969,22 +992,22 @@
         <v>23</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G8" s="6">
         <v>42198</v>
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>24</v>
@@ -993,55 +1016,55 @@
         <v>23</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G9" s="6">
         <v>42198</v>
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G10" s="6">
         <v>42198</v>
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G11" s="6">
         <v>42198</v>
@@ -1086,24 +1109,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G14" s="6">
         <v>42198</v>
@@ -1112,94 +1135,94 @@
     </row>
     <row r="15" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="6">
+        <v>42198</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="C16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="6">
+        <v>42198</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="6">
-        <v>42198</v>
-      </c>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="6">
-        <v>42198</v>
-      </c>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="E17" s="5" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G17" s="6">
         <v>42198</v>
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G18" s="6">
         <v>42198</v>
@@ -1244,24 +1267,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G21" s="6">
         <v>42198</v>
@@ -1273,19 +1296,19 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G22" s="6">
         <v>42198</v>
@@ -1296,19 +1319,19 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G23" s="6">
         <v>42198</v>
@@ -1349,22 +1372,22 @@
     </row>
     <row r="26" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G26" s="6">
         <v>42196</v>
@@ -1372,22 +1395,22 @@
     </row>
     <row r="27" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G27" s="6">
         <v>42197</v>
@@ -1395,22 +1418,22 @@
     </row>
     <row r="28" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G28" s="6">
         <v>42198</v>
@@ -1451,22 +1474,22 @@
     </row>
     <row r="31" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G31" s="6">
         <v>42198</v>
@@ -1474,22 +1497,22 @@
     </row>
     <row r="32" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G32" s="6">
         <v>42198</v>
@@ -1527,24 +1550,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>98</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G35" s="6">
         <v>42198</v>

</xml_diff>